<commit_message>
Missouri no Centro-Oeste, apenas
</commit_message>
<xml_diff>
--- a/Divisao_EUA.xlsx
+++ b/Divisao_EUA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorm\Desktop\FGV\4º Semestre\07 - Banco de Dados\Trabalho A2\USA_Flights_Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E205DBB-F1EB-40BB-99C2-31AC3862E89E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4380CAEF-2A7B-4B5A-BBC6-D78F9ABAC504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{294999EC-61D4-4DB0-B504-6249677FDDDA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
   <si>
     <t>Estado</t>
   </si>
@@ -360,16 +360,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -399,7 +391,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,9 +706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68004D20-8BDC-4C15-8385-2767194F5CFF}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -859,10 +853,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -870,10 +864,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -881,10 +875,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -892,10 +886,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -903,10 +897,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -914,21 +908,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -936,10 +930,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -947,10 +941,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -958,10 +952,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -969,10 +963,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -980,10 +974,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
@@ -991,10 +985,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -1002,10 +996,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -1013,10 +1007,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
@@ -1024,10 +1018,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -1035,10 +1029,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -1046,21 +1040,21 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
@@ -1068,10 +1062,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
@@ -1079,10 +1073,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -1090,10 +1084,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
         <v>33</v>
@@ -1101,10 +1095,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
@@ -1112,10 +1106,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
         <v>33</v>
@@ -1123,10 +1117,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -1134,10 +1128,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -1145,21 +1139,21 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
         <v>53</v>
@@ -1167,10 +1161,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
         <v>53</v>
@@ -1178,10 +1172,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
         <v>53</v>
@@ -1189,10 +1183,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>53</v>
@@ -1200,10 +1194,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
         <v>53</v>
@@ -1211,10 +1205,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
         <v>53</v>
@@ -1222,10 +1216,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
         <v>53</v>
@@ -1233,10 +1227,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
         <v>53</v>
@@ -1244,10 +1238,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
@@ -1255,10 +1249,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
         <v>53</v>
@@ -1266,10 +1260,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
         <v>53</v>
@@ -1277,23 +1271,12 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>